<commit_message>
Update the product backlog after the initial meeting
</commit_message>
<xml_diff>
--- a/backlog/product/product-backlog.xlsx
+++ b/backlog/product/product-backlog.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paolopenazzi/Desktop/pps-pvzlike/backlog/product/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB08EBA-A4FB-D045-B9AA-765F6A5D6764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,9 +24,83 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>Sprint 5</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Backlog Item</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Details (Wiki, URLs etc.)</t>
+  </si>
+  <si>
+    <t>Developers</t>
+  </si>
+  <si>
+    <t>Estimated Effort (1-10)</t>
+  </si>
+  <si>
+    <t>Effective Effort per Sprint</t>
+  </si>
+  <si>
+    <t>Knowledge Crunching</t>
+  </si>
+  <si>
+    <t>Understanding what the game is about</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Technology Analysis</t>
+  </si>
+  <si>
+    <t>Game Pattern Definition (MVC - GameLoop)</t>
+  </si>
+  <si>
+    <t>Domains understanding</t>
+  </si>
+  <si>
+    <t>Choose Domain Entities and their types</t>
+  </si>
+  <si>
+    <t>Continuous Integration</t>
+  </si>
+  <si>
+    <t>Studying Typical Approaches</t>
+  </si>
+  <si>
+    <t>Define ci Workflow</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +108,79 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCE4D6"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD6DCE4"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBF8F00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF548235"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FFE2EFDA"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -45,12 +188,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +516,279 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="25.5" customWidth="1"/>
+    <col min="3" max="3" width="34.83203125" customWidth="1"/>
+    <col min="4" max="4" width="30.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="6"/>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="7"/>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="11">
+        <v>1</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="12">
+        <v>6</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="11">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="2">
+        <v>6</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="11">
+        <v>3</v>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="12">
+        <v>3</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="11">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="2">
+        <v>4</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="11">
+        <v>5</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="12">
+        <v>3</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="11">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="2">
+        <v>6</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change java version to 1.16 because 1.17 is not presente
</commit_message>
<xml_diff>
--- a/backlog/product/product-backlog.xlsx
+++ b/backlog/product/product-backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paolopenazzi/Desktop/pps-pvzlike/backlog/product/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F56FAAB-A853-9B46-91E0-C60F42EF0730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B72616C-E7FF-384E-946D-BDAF755CF7DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -520,7 +520,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -782,7 +782,7 @@
         <v>14</v>
       </c>
       <c r="F14" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="13"/>

</xml_diff>

<commit_message>
Update product backlog. skip ci
</commit_message>
<xml_diff>
--- a/backlog/product/product-backlog.xlsx
+++ b/backlog/product/product-backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paolopenazzi/Desktop/pps-pvzlike/backlog/product/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B72616C-E7FF-384E-946D-BDAF755CF7DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{173D5AF2-5B07-3347-B57E-3C2A965427F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -94,6 +94,33 @@
   </si>
   <si>
     <t>Implement CI workflow</t>
+  </si>
+  <si>
+    <t>Turret</t>
+  </si>
+  <si>
+    <t>Enemy</t>
+  </si>
+  <si>
+    <t>Game Field</t>
+  </si>
+  <si>
+    <t>Game Loop</t>
+  </si>
+  <si>
+    <t>Penazzi</t>
+  </si>
+  <si>
+    <t>Parrinello</t>
+  </si>
+  <si>
+    <t>Alpi</t>
+  </si>
+  <si>
+    <t>Foschini</t>
+  </si>
+  <si>
+    <t>Game Entities</t>
   </si>
 </sst>
 </file>
@@ -124,7 +151,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,6 +204,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF2CC"/>
         <bgColor rgb="FFE2EFDA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor rgb="FFE2EFDA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -220,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -237,6 +282,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="131" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -528,7 +576,7 @@
     <col min="2" max="2" width="25.5" customWidth="1"/>
     <col min="3" max="3" width="46.6640625" customWidth="1"/>
     <col min="4" max="4" width="30.33203125" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.5" customWidth="1"/>
     <col min="6" max="6" width="18.6640625" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
@@ -789,6 +837,60 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B15" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B16" s="14"/>
+      <c r="C16" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="14"/>
+      <c r="C17" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="16"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="14">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Docs: Fix a typo in the product backlog. skip ci
</commit_message>
<xml_diff>
--- a/backlog/product/product-backlog.xlsx
+++ b/backlog/product/product-backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paolopenazzi/Desktop/pps-pvzlike/backlog/product/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{173D5AF2-5B07-3347-B57E-3C2A965427F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C5D8D1B-A6FC-0F44-86EB-D8CE34E4FF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -568,7 +568,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="131" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -838,6 +838,9 @@
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="11">
+        <v>7</v>
+      </c>
       <c r="B15" s="14" t="s">
         <v>31</v>
       </c>
@@ -853,6 +856,9 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="11">
+        <v>8</v>
+      </c>
       <c r="B16" s="14"/>
       <c r="C16" s="16" t="s">
         <v>24</v>
@@ -865,7 +871,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="11">
+        <v>9</v>
+      </c>
       <c r="B17" s="14"/>
       <c r="C17" s="15" t="s">
         <v>25</v>
@@ -878,7 +887,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="11">
+        <v>10</v>
+      </c>
       <c r="B18" s="14" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
product backlog updated after second sprint meeting
</commit_message>
<xml_diff>
--- a/backlog/product/product-backlog.xlsx
+++ b/backlog/product/product-backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paolopenazzi/Desktop/pps-pvzlike/backlog/product/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Desktop\UniBo\Primo Anno\PPS\Progetto\pps-pvzlike\backlog\product\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C5D8D1B-A6FC-0F44-86EB-D8CE34E4FF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D5AC42-05B1-4FBE-83D6-491A72E230DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -96,18 +96,9 @@
     <t>Implement CI workflow</t>
   </si>
   <si>
-    <t>Turret</t>
-  </si>
-  <si>
-    <t>Enemy</t>
-  </si>
-  <si>
     <t>Game Field</t>
   </si>
   <si>
-    <t>Game Loop</t>
-  </si>
-  <si>
     <t>Penazzi</t>
   </si>
   <si>
@@ -120,7 +111,31 @@
     <t>Foschini</t>
   </si>
   <si>
-    <t>Game Entities</t>
+    <t>First Model Game Entities</t>
+  </si>
+  <si>
+    <t>Turret's Properties</t>
+  </si>
+  <si>
+    <t>Enemy's Properties</t>
+  </si>
+  <si>
+    <t>First Game Loop</t>
+  </si>
+  <si>
+    <t>First Actor Game Entities</t>
+  </si>
+  <si>
+    <t>Turret's Actor</t>
+  </si>
+  <si>
+    <t>Enemy's Actor</t>
+  </si>
+  <si>
+    <t>First Game Rendering</t>
+  </si>
+  <si>
+    <t>Alpi, Parrinello</t>
   </si>
 </sst>
 </file>
@@ -151,7 +166,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,6 +237,18 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -265,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -285,9 +312,17 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -565,23 +600,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="131" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScale="64" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="25.5" customWidth="1"/>
-    <col min="3" max="3" width="46.6640625" customWidth="1"/>
-    <col min="4" max="4" width="30.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.5" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="1" max="1" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="8.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -595,7 +632,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -609,7 +646,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="3" t="s">
         <v>2</v>
@@ -623,7 +660,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="3" t="s">
         <v>3</v>
@@ -637,7 +674,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="3" t="s">
         <v>4</v>
@@ -651,7 +688,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -663,7 +700,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
@@ -689,7 +726,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -708,8 +745,11 @@
       <c r="J8" s="10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>1</v>
       </c>
@@ -726,14 +766,16 @@
       <c r="F9" s="12">
         <v>6</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1">
+        <v>6</v>
+      </c>
       <c r="H9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="11">
         <v>2</v>
       </c>
@@ -748,12 +790,14 @@
       <c r="F10" s="2">
         <v>6</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1">
+        <v>6</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
         <v>3</v>
       </c>
@@ -768,12 +812,14 @@
       <c r="F11" s="12">
         <v>3</v>
       </c>
-      <c r="G11" s="1"/>
+      <c r="G11" s="1">
+        <v>3</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <v>4</v>
       </c>
@@ -790,12 +836,14 @@
       <c r="F12" s="2">
         <v>1</v>
       </c>
-      <c r="G12" s="1"/>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
         <v>5</v>
       </c>
@@ -812,12 +860,14 @@
       <c r="F13" s="12">
         <v>3</v>
       </c>
-      <c r="G13" s="1"/>
+      <c r="G13" s="1">
+        <v>3</v>
+      </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="11">
         <v>6</v>
       </c>
@@ -832,75 +882,137 @@
       <c r="F14" s="2">
         <v>5</v>
       </c>
-      <c r="G14" s="1"/>
+      <c r="G14" s="1">
+        <v>5</v>
+      </c>
       <c r="H14" s="13"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
         <v>7</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F15" s="14">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="11">
         <v>8</v>
       </c>
       <c r="B16" s="14"/>
       <c r="C16" s="16" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F16" s="14">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="11">
         <v>9</v>
       </c>
       <c r="B17" s="14"/>
       <c r="C17" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D17" s="14"/>
       <c r="E17" s="14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F17" s="14">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="11">
         <v>10</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F18" s="14">
         <v>8</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="19">
+        <v>11</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="20"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="19">
+        <v>12</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="18">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
doc: update product-backlog with Sprint-3 backlog items
</commit_message>
<xml_diff>
--- a/backlog/product/product-backlog.xlsx
+++ b/backlog/product/product-backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Desktop\UniBo\Primo Anno\PPS\Progetto\pps-pvzlike\backlog\product\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D5AC42-05B1-4FBE-83D6-491A72E230DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF1BA1C-8FA8-4379-8DD1-40DD75D90362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="78">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Implement CI workflow</t>
   </si>
   <si>
-    <t>Game Field</t>
-  </si>
-  <si>
     <t>Penazzi</t>
   </si>
   <si>
@@ -123,19 +120,145 @@
     <t>First Game Loop</t>
   </si>
   <si>
-    <t>First Actor Game Entities</t>
-  </si>
-  <si>
-    <t>Turret's Actor</t>
-  </si>
-  <si>
     <t>Enemy's Actor</t>
   </si>
   <si>
-    <t>First Game Rendering</t>
-  </si>
-  <si>
-    <t>Alpi, Parrinello</t>
+    <t>Create initial GameLoop Actor</t>
+  </si>
+  <si>
+    <t>Which messages Actors should have</t>
+  </si>
+  <si>
+    <t>First Turret's Actor</t>
+  </si>
+  <si>
+    <t>Fire Logic</t>
+  </si>
+  <si>
+    <t>Bullet Spawning</t>
+  </si>
+  <si>
+    <t>Bullet's Properties</t>
+  </si>
+  <si>
+    <t>Collision: how they should be</t>
+  </si>
+  <si>
+    <t>ScalaFX VS LibGDX (yet another technology analysis)</t>
+  </si>
+  <si>
+    <t>Hello world with both tech</t>
+  </si>
+  <si>
+    <t>Studying LibGDX documentation</t>
+  </si>
+  <si>
+    <t>Define Update and Start Phase</t>
+  </si>
+  <si>
+    <t>Create initial Launcher and its Root Actor</t>
+  </si>
+  <si>
+    <t>Figure out how many behaviors should have GameLoop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implements the Root's Actor behaviors </t>
+  </si>
+  <si>
+    <t>First Implementation of WaveSupervisor</t>
+  </si>
+  <si>
+    <t>First WaveSupervisor</t>
+  </si>
+  <si>
+    <t>Immutability of Entities</t>
+  </si>
+  <si>
+    <t>Introduce the immutability in entity's creation phase</t>
+  </si>
+  <si>
+    <t>Standard Model Messages</t>
+  </si>
+  <si>
+    <t>Introduce a Standard for Model Messages</t>
+  </si>
+  <si>
+    <t>Penazzi, Parrinello</t>
+  </si>
+  <si>
+    <t>First View Actor</t>
+  </si>
+  <si>
+    <t>Implements an easy View Actor for the first release</t>
+  </si>
+  <si>
+    <t>Collision Handling</t>
+  </si>
+  <si>
+    <t>Implements a meccanish for the collision between the entities</t>
+  </si>
+  <si>
+    <t>GameField Rendering</t>
+  </si>
+  <si>
+    <t>Render the whole game including the field sprites</t>
+  </si>
+  <si>
+    <t>Mana Modelling</t>
+  </si>
+  <si>
+    <t>Study how the Mana/Sun should increase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implements the Mana/Sun Model </t>
+  </si>
+  <si>
+    <t>Implements the interaction with Mana Model and Controller</t>
+  </si>
+  <si>
+    <t>Wave Modelling</t>
+  </si>
+  <si>
+    <t>Implements the Model behing the Wave concept</t>
+  </si>
+  <si>
+    <t>How Wave interact with GameLoop</t>
+  </si>
+  <si>
+    <t>Whole Game Interface</t>
+  </si>
+  <si>
+    <t>Create the view interface for the match</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entity State concept </t>
+  </si>
+  <si>
+    <t>Introduce a state concept in each entities</t>
+  </si>
+  <si>
+    <t>View refactor</t>
+  </si>
+  <si>
+    <t>View code refactor</t>
+  </si>
+  <si>
+    <t>Architecture refactor</t>
+  </si>
+  <si>
+    <t>Reduce HW Request</t>
+  </si>
+  <si>
+    <t>Figure out why the system is so HW intense</t>
+  </si>
+  <si>
+    <t>Wave Prolog</t>
+  </si>
+  <si>
+    <t>Use Prolog Engine to create Waves</t>
+  </si>
+  <si>
+    <t>Parrinello, Penazzi</t>
   </si>
 </sst>
 </file>
@@ -166,7 +289,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,8 +374,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -288,11 +417,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -319,6 +459,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -600,21 +752,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="64" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
     <col min="8" max="11" width="8.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -894,14 +1046,14 @@
         <v>7</v>
       </c>
       <c r="B15" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>28</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>29</v>
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F15" s="14">
         <v>4</v>
@@ -911,108 +1063,539 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="11">
-        <v>8</v>
-      </c>
+      <c r="A16" s="11"/>
       <c r="B16" s="14"/>
-      <c r="C16" s="16" t="s">
-        <v>30</v>
+      <c r="C16" s="15" t="s">
+        <v>37</v>
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="14" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F16" s="14">
         <v>4</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" s="14"/>
-      <c r="C17" s="15" t="s">
-        <v>23</v>
+      <c r="C17" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="D17" s="14"/>
       <c r="E17" s="14" t="s">
         <v>26</v>
       </c>
       <c r="F17" s="14">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="16"/>
+        <v>30</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>32</v>
+      </c>
       <c r="D18" s="14"/>
       <c r="E18" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F18" s="14">
-        <v>8</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="19">
-        <v>11</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="11">
+        <v>9</v>
+      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="18">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
-      <c r="B20" s="18"/>
+      <c r="F19" s="14">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="19">
+        <v>10</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>34</v>
+      </c>
       <c r="C20" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D20" s="18"/>
       <c r="E20" s="18" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F20" s="18">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="19">
-        <v>12</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="18"/>
+        <v>5</v>
+      </c>
+      <c r="H20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="19"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="D21" s="18"/>
       <c r="E21" s="18" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F21" s="18">
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="20"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="18">
+        <v>6</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="19">
+        <v>11</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="18">
+        <v>4</v>
+      </c>
+      <c r="H23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="19">
+        <v>12</v>
+      </c>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="18">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="22">
+        <v>13</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="24"/>
+      <c r="E25" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="21">
+        <v>5</v>
+      </c>
+      <c r="H25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="19"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="18">
+        <v>6</v>
+      </c>
+      <c r="H26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="19"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="18">
+        <v>3</v>
+      </c>
+      <c r="H27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="23">
+        <v>16</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="18">
+        <v>2</v>
+      </c>
+      <c r="H28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="19">
+        <v>17</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" s="18">
+        <v>2</v>
+      </c>
+      <c r="H29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="19">
+        <v>18</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="18">
+        <v>5</v>
+      </c>
+      <c r="H30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="23">
+        <v>19</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F31" s="18">
+        <v>3</v>
+      </c>
+      <c r="H31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="19">
+        <v>20</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" s="18">
+        <v>3</v>
+      </c>
+      <c r="H32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="19">
+        <v>21</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="26">
+        <v>22</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="25"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="26">
+        <v>23</v>
+      </c>
+      <c r="B35" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="19"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F36" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="19"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F37" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="26">
+        <v>24</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38" s="25"/>
+      <c r="E38" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="F38" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="19"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="F39" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="19">
+        <v>25</v>
+      </c>
+      <c r="B40" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40" s="25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="19">
+        <v>26</v>
+      </c>
+      <c r="B41" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" s="25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="19">
+        <v>27</v>
+      </c>
+      <c r="B42" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D42" s="25"/>
+      <c r="E42" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="19">
+        <v>28</v>
+      </c>
+      <c r="B43" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C43" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="19">
+        <v>29</v>
+      </c>
+      <c r="B44" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D44" s="25"/>
+      <c r="E44" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="F44" s="25">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs: update product-backolg with fourth-sprint's backlog items
</commit_message>
<xml_diff>
--- a/backlog/product/product-backlog.xlsx
+++ b/backlog/product/product-backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Desktop\UniBo\Primo Anno\PPS\Progetto\pps-pvzlike\backlog\product\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF1BA1C-8FA8-4379-8DD1-40DD75D90362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83E465F-1C1F-4F4E-A621-A1DA53FC6F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="103">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -108,18 +108,12 @@
     <t>Foschini</t>
   </si>
   <si>
-    <t>First Model Game Entities</t>
-  </si>
-  <si>
     <t>Turret's Properties</t>
   </si>
   <si>
     <t>Enemy's Properties</t>
   </si>
   <si>
-    <t>First Game Loop</t>
-  </si>
-  <si>
     <t>Enemy's Actor</t>
   </si>
   <si>
@@ -219,9 +213,6 @@
     <t>Wave Modelling</t>
   </si>
   <si>
-    <t>Implements the Model behing the Wave concept</t>
-  </si>
-  <si>
     <t>How Wave interact with GameLoop</t>
   </si>
   <si>
@@ -237,12 +228,6 @@
     <t>Introduce a state concept in each entities</t>
   </si>
   <si>
-    <t>View refactor</t>
-  </si>
-  <si>
-    <t>View code refactor</t>
-  </si>
-  <si>
     <t>Architecture refactor</t>
   </si>
   <si>
@@ -259,6 +244,96 @@
   </si>
   <si>
     <t>Parrinello, Penazzi</t>
+  </si>
+  <si>
+    <t>Implements the Model behind the Wave concept</t>
+  </si>
+  <si>
+    <t>Cells logic</t>
+  </si>
+  <si>
+    <t>Add cells logic to viewport</t>
+  </si>
+  <si>
+    <t>Add click listeners to cards and cells to place turrets</t>
+  </si>
+  <si>
+    <t>Model Game Entities</t>
+  </si>
+  <si>
+    <t>Game Loop</t>
+  </si>
+  <si>
+    <t>Make Troop Actor</t>
+  </si>
+  <si>
+    <t>Create Troop Actor</t>
+  </si>
+  <si>
+    <t>Introduce the concept of Troop in the Entity Model</t>
+  </si>
+  <si>
+    <t>Foschini, Penazzi</t>
+  </si>
+  <si>
+    <t>New troop entity types</t>
+  </si>
+  <si>
+    <t>Introduce new types of troop</t>
+  </si>
+  <si>
+    <t>End match view</t>
+  </si>
+  <si>
+    <t>Render the end match view</t>
+  </si>
+  <si>
+    <t>Add statistics</t>
+  </si>
+  <si>
+    <t>Start match view</t>
+  </si>
+  <si>
+    <t>Render the start match view</t>
+  </si>
+  <si>
+    <t>Add button for select difficulty</t>
+  </si>
+  <si>
+    <t>Add button for start the match</t>
+  </si>
+  <si>
+    <t>In-game buttons</t>
+  </si>
+  <si>
+    <t>Add pause button</t>
+  </si>
+  <si>
+    <t>Add resume button</t>
+  </si>
+  <si>
+    <t>Add change game velocity button</t>
+  </si>
+  <si>
+    <t>Alpi, Foschini</t>
+  </si>
+  <si>
+    <t>Graphics Polish</t>
+  </si>
+  <si>
+    <t>Correct the position bullet height</t>
+  </si>
+  <si>
+    <t>Increase assets quality</t>
+  </si>
+  <si>
+    <t>Refactor of turrets placement position</t>
+  </si>
+  <si>
+    <t>Entity Animations</t>
+  </si>
+  <si>
+    <t>Render animations for each type of entity</t>
   </si>
 </sst>
 </file>
@@ -289,7 +364,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -376,12 +451,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -428,11 +509,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -468,8 +558,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -752,10 +847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1046,27 +1141,30 @@
         <v>7</v>
       </c>
       <c r="B15" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>27</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>28</v>
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="14" t="s">
         <v>23</v>
       </c>
       <c r="F15" s="14">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G15">
         <v>4</v>
+      </c>
+      <c r="I15">
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="14"/>
       <c r="C16" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="14" t="s">
@@ -1079,13 +1177,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="11">
         <v>8</v>
       </c>
       <c r="B17" s="14"/>
       <c r="C17" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" s="14"/>
       <c r="E17" s="14" t="s">
@@ -1100,16 +1198,19 @@
       <c r="H17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="11">
         <v>9</v>
       </c>
       <c r="B18" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="16" t="s">
         <v>30</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>32</v>
       </c>
       <c r="D18" s="14"/>
       <c r="E18" s="14" t="s">
@@ -1122,13 +1223,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="11">
         <v>9</v>
       </c>
       <c r="B19" s="14"/>
       <c r="C19" s="16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D19" s="14"/>
       <c r="E19" s="14" t="s">
@@ -1141,15 +1242,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="19">
         <v>10</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D20" s="18"/>
       <c r="E20" s="18" t="s">
@@ -1162,11 +1263,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="19"/>
       <c r="B21" s="18"/>
       <c r="C21" s="18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D21" s="18"/>
       <c r="E21" s="18" t="s">
@@ -1179,11 +1280,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="20"/>
       <c r="B22" s="18"/>
       <c r="C22" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D22" s="18"/>
       <c r="E22" s="18" t="s">
@@ -1195,16 +1296,19 @@
       <c r="H22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="19">
         <v>11</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="18" t="s">
@@ -1217,13 +1321,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="19">
         <v>12</v>
       </c>
       <c r="B24" s="18"/>
       <c r="C24" s="18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D24" s="18"/>
       <c r="E24" s="18" t="s">
@@ -1236,15 +1340,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="22">
         <v>13</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D25" s="24"/>
       <c r="E25" s="21" t="s">
@@ -1257,11 +1361,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="18"/>
       <c r="C26" s="18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="18" t="s">
@@ -1274,11 +1378,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
       <c r="B27" s="18"/>
       <c r="C27" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D27" s="18"/>
       <c r="E27" s="18" t="s">
@@ -1291,15 +1395,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="23">
         <v>16</v>
       </c>
       <c r="B28" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="18" t="s">
         <v>43</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>45</v>
       </c>
       <c r="D28" s="18"/>
       <c r="E28" s="18" t="s">
@@ -1312,15 +1416,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="19">
         <v>17</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D29" s="18"/>
       <c r="E29" s="18" t="s">
@@ -1333,15 +1437,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="19">
         <v>18</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D30" s="18"/>
       <c r="E30" s="18" t="s">
@@ -1354,19 +1458,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="23">
         <v>19</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F31" s="18">
         <v>3</v>
@@ -1375,15 +1479,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="19">
         <v>20</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="18" t="s">
@@ -1396,206 +1500,502 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="19">
         <v>21</v>
       </c>
-      <c r="B33" s="25" t="s">
+      <c r="B33" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="27">
+        <v>4</v>
+      </c>
+      <c r="I33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="19">
+        <v>22</v>
+      </c>
+      <c r="B34" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="25" t="s">
+      <c r="C34" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25" t="s">
+      <c r="D34" s="27"/>
+      <c r="E34" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="27">
+        <v>3</v>
+      </c>
+      <c r="I34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="19">
+        <v>23</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="F33" s="25">
+      <c r="F35" s="27">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="19"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="F36" s="27">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="26">
-        <v>22</v>
-      </c>
-      <c r="B34" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="F34" s="25"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="26">
+      <c r="I36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="19"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="F37" s="27">
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="19">
+        <v>24</v>
+      </c>
+      <c r="B38" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="F35" s="25">
+      <c r="F38" s="27">
+        <v>3</v>
+      </c>
+      <c r="I38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="19"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F39" s="27">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="19"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="F36" s="25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="19"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="F37" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="26">
-        <v>24</v>
-      </c>
-      <c r="B38" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C38" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="F38" s="25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="19"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="F39" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="19">
         <v>25</v>
       </c>
-      <c r="B40" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="C40" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25" t="s">
+      <c r="B40" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C40" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="F40" s="25">
+      <c r="F40" s="27">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="19">
         <v>26</v>
       </c>
-      <c r="B41" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="C41" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25" t="s">
+      <c r="B41" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C41" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="F41" s="25">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F41" s="27">
+        <v>2</v>
+      </c>
+      <c r="I41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="19">
         <v>27</v>
       </c>
-      <c r="B42" s="25" t="s">
+      <c r="B42" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" s="27">
+        <v>3</v>
+      </c>
+      <c r="I42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="19"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" s="27">
+        <v>3</v>
+      </c>
+      <c r="I43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="19">
+        <v>28</v>
+      </c>
+      <c r="B44" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C44" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44" s="27">
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="19">
+        <v>29</v>
+      </c>
+      <c r="B45" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="C42" s="25" t="s">
+      <c r="C45" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25" t="s">
+      <c r="D45" s="27"/>
+      <c r="E45" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="F45" s="27">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="19">
+        <v>30</v>
+      </c>
+      <c r="B46" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="D46" s="27"/>
+      <c r="E46" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="F46" s="27">
+        <v>3</v>
+      </c>
+      <c r="I46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="19"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="F47" s="27">
+        <v>3</v>
+      </c>
+      <c r="I47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" s="19">
+        <v>31</v>
+      </c>
+      <c r="B48" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C48" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="F48" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="19">
+        <v>32</v>
+      </c>
+      <c r="B49" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C49" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F49" s="26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="19"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F50" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="29">
+        <v>33</v>
+      </c>
+      <c r="B51" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C51" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F51" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="28"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F52" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="28"/>
+      <c r="B53" s="26"/>
+      <c r="C53" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="D53" s="26"/>
+      <c r="E53" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F53" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="28">
+        <v>34</v>
+      </c>
+      <c r="B54" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C54" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="F54" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="28"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="F55" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="28"/>
+      <c r="B56" s="26"/>
+      <c r="C56" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="F56" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="28">
+        <v>35</v>
+      </c>
+      <c r="B57" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C57" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="D57" s="26"/>
+      <c r="E57" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F42" s="25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="19">
-        <v>28</v>
-      </c>
-      <c r="B43" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="C43" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25" t="s">
+      <c r="F57" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="28"/>
+      <c r="B58" s="26"/>
+      <c r="C58" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="D58" s="26"/>
+      <c r="E58" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F43" s="25">
+      <c r="F58" s="26">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="19">
-        <v>29</v>
-      </c>
-      <c r="B44" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="C44" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="F44" s="25">
-        <v>8</v>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="28"/>
+      <c r="B59" s="26"/>
+      <c r="C59" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="D59" s="26"/>
+      <c r="E59" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F59" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="28">
+        <v>36</v>
+      </c>
+      <c r="B60" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="C60" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D60" s="26"/>
+      <c r="E60" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="F60" s="26">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs: update product backlog fourth-sprint. Update product backlg with fourth-sprint's effort and fifth-sprint's tasks
</commit_message>
<xml_diff>
--- a/backlog/product/product-backlog.xlsx
+++ b/backlog/product/product-backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Desktop\UniBo\Primo Anno\PPS\Progetto\pps-pvzlike\backlog\product\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83E465F-1C1F-4F4E-A621-A1DA53FC6F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDAC4DE-35F4-43F6-B68D-BD0BF6348E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="112">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -237,12 +237,6 @@
     <t>Figure out why the system is so HW intense</t>
   </si>
   <si>
-    <t>Wave Prolog</t>
-  </si>
-  <si>
-    <t>Use Prolog Engine to create Waves</t>
-  </si>
-  <si>
     <t>Parrinello, Penazzi</t>
   </si>
   <si>
@@ -297,9 +291,6 @@
     <t>Render the start match view</t>
   </si>
   <si>
-    <t>Add button for select difficulty</t>
-  </si>
-  <si>
     <t>Add button for start the match</t>
   </si>
   <si>
@@ -334,6 +325,42 @@
   </si>
   <si>
     <t>Render animations for each type of entity</t>
+  </si>
+  <si>
+    <t>Penazzi, Foschini</t>
+  </si>
+  <si>
+    <t>Make Prolog</t>
+  </si>
+  <si>
+    <t>Make Prolog Theory but without the integration</t>
+  </si>
+  <si>
+    <t>Integration Prolog</t>
+  </si>
+  <si>
+    <t>Prolog-Scala Integration in order to create random wave</t>
+  </si>
+  <si>
+    <t>Docs review</t>
+  </si>
+  <si>
+    <t>Reviews all documentations and correct little things</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Fix bugs</t>
+  </si>
+  <si>
+    <t>Fix little bug around the whole game</t>
+  </si>
+  <si>
+    <t>Increase usability</t>
+  </si>
+  <si>
+    <t>Increase usability introducing new buttons, align the text, ecc.</t>
   </si>
 </sst>
 </file>
@@ -364,7 +391,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -461,6 +488,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -522,7 +555,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -558,15 +591,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -847,10 +883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K60"/>
+  <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1141,7 +1177,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>27</v>
@@ -1168,13 +1204,16 @@
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="14" t="s">
-        <v>23</v>
+        <v>100</v>
       </c>
       <c r="F16" s="14">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G16" s="1">
         <v>4</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1198,7 +1237,7 @@
       <c r="H17">
         <v>1</v>
       </c>
-      <c r="I17" s="25">
+      <c r="I17">
         <v>2</v>
       </c>
     </row>
@@ -1207,7 +1246,7 @@
         <v>9</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>30</v>
@@ -1500,502 +1539,578 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="19">
         <v>21</v>
       </c>
-      <c r="B33" s="27" t="s">
+      <c r="B33" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C33" s="27" t="s">
+      <c r="C33" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27" t="s">
+      <c r="D33" s="26"/>
+      <c r="E33" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="F33" s="27">
+      <c r="F33" s="26">
         <v>4</v>
       </c>
       <c r="I33">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="19">
         <v>22</v>
       </c>
-      <c r="B34" s="27" t="s">
+      <c r="B34" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="27" t="s">
+      <c r="C34" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27" t="s">
+      <c r="D34" s="26"/>
+      <c r="E34" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="F34" s="27">
+      <c r="F34" s="26">
         <v>3</v>
       </c>
       <c r="I34">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="19">
         <v>23</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="C35" s="27" t="s">
+      <c r="C35" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27" t="s">
+      <c r="D35" s="26"/>
+      <c r="E35" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="F35" s="27">
+      <c r="F35" s="26">
         <v>1</v>
       </c>
       <c r="I35">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="19"/>
-      <c r="B36" s="27"/>
-      <c r="C36" s="27" t="s">
+      <c r="B36" s="26"/>
+      <c r="C36" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27" t="s">
+      <c r="D36" s="26"/>
+      <c r="E36" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="F36" s="27">
+      <c r="F36" s="26">
         <v>4</v>
       </c>
       <c r="I36">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="19"/>
-      <c r="B37" s="27"/>
-      <c r="C37" s="27" t="s">
+      <c r="B37" s="26"/>
+      <c r="C37" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="27"/>
-      <c r="E37" s="27" t="s">
+      <c r="D37" s="26"/>
+      <c r="E37" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="F37" s="27">
+      <c r="F37" s="26">
         <v>2</v>
       </c>
       <c r="I37">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="19">
         <v>24</v>
       </c>
-      <c r="B38" s="27" t="s">
+      <c r="B38" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="C38" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="D38" s="27"/>
-      <c r="E38" s="27" t="s">
+      <c r="C38" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="F38" s="27">
+      <c r="F38" s="26">
         <v>3</v>
       </c>
       <c r="I38">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="19"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="27" t="s">
+      <c r="B39" s="26"/>
+      <c r="C39" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27" t="s">
+      <c r="D39" s="26"/>
+      <c r="E39" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="F39" s="27">
+      <c r="F39" s="26">
         <v>1</v>
       </c>
       <c r="I39">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="19">
         <v>25</v>
       </c>
-      <c r="B40" s="27" t="s">
+      <c r="B40" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="C40" s="27" t="s">
+      <c r="C40" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27" t="s">
+      <c r="D40" s="26"/>
+      <c r="E40" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="F40" s="27">
+      <c r="F40" s="26">
         <v>6</v>
       </c>
       <c r="I40">
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="19">
         <v>26</v>
       </c>
-      <c r="B41" s="27" t="s">
+      <c r="B41" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="C41" s="27" t="s">
+      <c r="C41" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27" t="s">
+      <c r="D41" s="26"/>
+      <c r="E41" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F41" s="27">
+      <c r="F41" s="26">
         <v>2</v>
       </c>
       <c r="I41">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="19">
         <v>27</v>
       </c>
-      <c r="B42" s="27" t="s">
+      <c r="B42" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" s="26">
+        <v>3</v>
+      </c>
+      <c r="I42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="19"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="C42" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="D42" s="27"/>
-      <c r="E42" s="27" t="s">
+      <c r="D43" s="26"/>
+      <c r="E43" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F42" s="27">
-        <v>3</v>
-      </c>
-      <c r="I42">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="19"/>
-      <c r="B43" s="27"/>
-      <c r="C43" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="F43" s="27">
+      <c r="F43" s="26">
         <v>3</v>
       </c>
       <c r="I43">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="19">
         <v>28</v>
       </c>
-      <c r="B44" s="27" t="s">
+      <c r="B44" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="C44" s="27" t="s">
+      <c r="C44" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="D44" s="27"/>
-      <c r="E44" s="27" t="s">
+      <c r="D44" s="26"/>
+      <c r="E44" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F44" s="27">
+      <c r="F44" s="26">
         <v>1</v>
       </c>
       <c r="I44">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="19">
         <v>29</v>
       </c>
-      <c r="B45" s="27" t="s">
+      <c r="B45" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="C45" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="D45" s="27"/>
-      <c r="E45" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="F45" s="27">
+      <c r="F45" s="26">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="19">
         <v>30</v>
       </c>
-      <c r="B46" s="27" t="s">
+      <c r="B46" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F46" s="26">
+        <v>3</v>
+      </c>
+      <c r="I46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="19"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="C46" s="27" t="s">
+      <c r="D47" s="26"/>
+      <c r="E47" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="D46" s="27"/>
-      <c r="E46" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="F46" s="27">
-        <v>3</v>
-      </c>
-      <c r="I46">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="19"/>
-      <c r="B47" s="27"/>
-      <c r="C47" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="F47" s="27">
+      <c r="F47" s="26">
         <v>3</v>
       </c>
       <c r="I47">
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="19">
         <v>31</v>
       </c>
-      <c r="B48" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="C48" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26" t="s">
+      <c r="B48" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="F48" s="26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D48" s="25"/>
+      <c r="E48" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="F48" s="25">
+        <v>2</v>
+      </c>
+      <c r="J48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="19">
         <v>32</v>
       </c>
-      <c r="B49" s="26" t="s">
+      <c r="B49" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F49" s="25">
+        <v>6</v>
+      </c>
+      <c r="J49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="19"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="C49" s="26" t="s">
+      <c r="D50" s="25"/>
+      <c r="E50" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F50" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="28">
+        <v>33</v>
+      </c>
+      <c r="B51" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="F49" s="26">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="19"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="26" t="s">
+      <c r="C51" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="D50" s="26"/>
-      <c r="E50" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="F50" s="26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="29">
-        <v>33</v>
-      </c>
-      <c r="B51" s="26" t="s">
+      <c r="D51" s="25"/>
+      <c r="E51" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F51" s="25">
+        <v>2</v>
+      </c>
+      <c r="J51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="27"/>
+      <c r="B52" s="25"/>
+      <c r="C52" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="C51" s="26" t="s">
+      <c r="D52" s="25"/>
+      <c r="E52" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F52" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" s="27">
+        <v>34</v>
+      </c>
+      <c r="B53" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26" t="s">
+      <c r="C53" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="D53" s="25"/>
+      <c r="E53" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="F53" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" s="27"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="D54" s="25"/>
+      <c r="E54" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="F54" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55" s="27"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="F55" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" s="27">
+        <v>35</v>
+      </c>
+      <c r="B56" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C56" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D56" s="25"/>
+      <c r="E56" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F56" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57" s="27"/>
+      <c r="B57" s="25"/>
+      <c r="C57" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="D57" s="25"/>
+      <c r="E57" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F57" s="25">
+        <v>1</v>
+      </c>
+      <c r="J57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A58" s="27"/>
+      <c r="B58" s="25"/>
+      <c r="C58" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="D58" s="25"/>
+      <c r="E58" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F58" s="25">
+        <v>2</v>
+      </c>
+      <c r="J58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59" s="27">
+        <v>36</v>
+      </c>
+      <c r="B59" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="C59" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="D59" s="25"/>
+      <c r="E59" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="F59" s="25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60" s="22">
+        <v>37</v>
+      </c>
+      <c r="B60" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="C60" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="D60" s="30"/>
+      <c r="E60" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="F60" s="30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61" s="29">
+        <v>38</v>
+      </c>
+      <c r="B61" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="C61" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="D61" s="30"/>
+      <c r="E61" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="F61" s="30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A62" s="29">
+        <v>39</v>
+      </c>
+      <c r="B62" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="C62" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="D62" s="30"/>
+      <c r="E62" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="F62" s="30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A63" s="29">
+        <v>40</v>
+      </c>
+      <c r="B63" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="C63" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="D63" s="30"/>
+      <c r="E63" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="F51" s="26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="28"/>
-      <c r="B52" s="26"/>
-      <c r="C52" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="D52" s="26"/>
-      <c r="E52" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="F52" s="26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="28"/>
-      <c r="B53" s="26"/>
-      <c r="C53" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="D53" s="26"/>
-      <c r="E53" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="F53" s="26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="28">
-        <v>34</v>
-      </c>
-      <c r="B54" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="C54" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="D54" s="26"/>
-      <c r="E54" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="F54" s="26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="28"/>
-      <c r="B55" s="26"/>
-      <c r="C55" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="D55" s="26"/>
-      <c r="E55" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="F55" s="26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="28"/>
-      <c r="B56" s="26"/>
-      <c r="C56" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="D56" s="26"/>
-      <c r="E56" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="F56" s="26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="28">
-        <v>35</v>
-      </c>
-      <c r="B57" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="C57" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="D57" s="26"/>
-      <c r="E57" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="F57" s="26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="28"/>
-      <c r="B58" s="26"/>
-      <c r="C58" s="26" t="s">
-        <v>99</v>
-      </c>
-      <c r="D58" s="26"/>
-      <c r="E58" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="F58" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="28"/>
-      <c r="B59" s="26"/>
-      <c r="C59" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="D59" s="26"/>
-      <c r="E59" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="F59" s="26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="28">
-        <v>36</v>
-      </c>
-      <c r="B60" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="C60" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="D60" s="26"/>
-      <c r="E60" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="F60" s="26">
-        <v>5</v>
+      <c r="F63" s="30">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs: add fifth sprint review
</commit_message>
<xml_diff>
--- a/backlog/product/product-backlog.xlsx
+++ b/backlog/product/product-backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Desktop\UniBo\Primo Anno\PPS\Progetto\pps-pvzlike\backlog\product\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paolopenazzi/Desktop/pps-pvzlike/backlog/product/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDAC4DE-35F4-43F6-B68D-BD0BF6348E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BA54C6-1B19-9C45-90F2-92C71B8D4A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="112">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -321,12 +321,6 @@
     <t>Refactor of turrets placement position</t>
   </si>
   <si>
-    <t>Entity Animations</t>
-  </si>
-  <si>
-    <t>Render animations for each type of entity</t>
-  </si>
-  <si>
     <t>Penazzi, Foschini</t>
   </si>
   <si>
@@ -361,6 +355,12 @@
   </si>
   <si>
     <t>Increase usability introducing new buttons, align the text, ecc.</t>
+  </si>
+  <si>
+    <t>Alpi, Parrinello</t>
+  </si>
+  <si>
+    <t>Add fade animation</t>
   </si>
 </sst>
 </file>
@@ -605,7 +605,7 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -885,23 +885,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K63" sqref="K63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -915,7 +915,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -929,7 +929,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="3" t="s">
         <v>2</v>
@@ -943,7 +943,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
       <c r="B4" s="3" t="s">
         <v>3</v>
@@ -957,7 +957,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="3" t="s">
         <v>4</v>
@@ -971,7 +971,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -983,7 +983,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
@@ -1009,7 +1009,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1032,7 +1032,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>1</v>
       </c>
@@ -1058,7 +1058,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>2</v>
       </c>
@@ -1080,7 +1080,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>3</v>
       </c>
@@ -1102,7 +1102,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>4</v>
       </c>
@@ -1126,7 +1126,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>5</v>
       </c>
@@ -1150,7 +1150,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
         <v>6</v>
       </c>
@@ -1172,7 +1172,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
         <v>7</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="14"/>
       <c r="C16" s="15" t="s">
@@ -1204,7 +1204,7 @@
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F16" s="14">
         <v>6</v>
@@ -1216,7 +1216,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>8</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>9</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>9</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="19">
         <v>10</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="19"/>
       <c r="B21" s="18"/>
       <c r="C21" s="18" t="s">
@@ -1319,7 +1319,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="20"/>
       <c r="B22" s="18"/>
       <c r="C22" s="18" t="s">
@@ -1339,7 +1339,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="19">
         <v>11</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="19">
         <v>12</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="22">
         <v>13</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="19"/>
       <c r="B26" s="18"/>
       <c r="C26" s="18" t="s">
@@ -1417,7 +1417,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="19"/>
       <c r="B27" s="18"/>
       <c r="C27" s="18" t="s">
@@ -1434,7 +1434,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="23">
         <v>16</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="19">
         <v>17</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="19">
         <v>18</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="23">
         <v>19</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="19">
         <v>20</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="19">
         <v>21</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="19">
         <v>22</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="19">
         <v>23</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="19"/>
       <c r="B36" s="26"/>
       <c r="C36" s="26" t="s">
@@ -1619,7 +1619,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="19"/>
       <c r="B37" s="26"/>
       <c r="C37" s="26" t="s">
@@ -1636,7 +1636,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="19">
         <v>24</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="19"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26" t="s">
@@ -1674,7 +1674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="19">
         <v>25</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="19">
         <v>26</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="19">
         <v>27</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="19"/>
       <c r="B43" s="26"/>
       <c r="C43" s="26" t="s">
@@ -1754,7 +1754,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="19">
         <v>28</v>
       </c>
@@ -1775,15 +1775,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="19">
         <v>29</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C45" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D45" s="26"/>
       <c r="E45" s="26" t="s">
@@ -1796,7 +1796,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="19">
         <v>30</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="19"/>
       <c r="B47" s="26"/>
       <c r="C47" s="26" t="s">
@@ -1834,7 +1834,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="19">
         <v>31</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="19">
         <v>32</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="19"/>
       <c r="B50" s="25"/>
       <c r="C50" s="25" t="s">
@@ -1890,7 +1890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="28">
         <v>33</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="27"/>
       <c r="B52" s="25"/>
       <c r="C52" s="25" t="s">
@@ -1924,8 +1924,11 @@
       <c r="F52" s="25">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="27">
         <v>34</v>
       </c>
@@ -1942,8 +1945,11 @@
       <c r="F53" s="25">
         <v>2</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K53">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="27"/>
       <c r="B54" s="25"/>
       <c r="C54" s="25" t="s">
@@ -1956,8 +1962,11 @@
       <c r="F54" s="25">
         <v>2</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="27"/>
       <c r="B55" s="25"/>
       <c r="C55" s="25" t="s">
@@ -1970,8 +1979,11 @@
       <c r="F55" s="25">
         <v>2</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K55">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="27">
         <v>35</v>
       </c>
@@ -1988,8 +2000,11 @@
       <c r="F56" s="25">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="27"/>
       <c r="B57" s="25"/>
       <c r="C57" s="25" t="s">
@@ -2006,7 +2021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="27"/>
       <c r="B58" s="25"/>
       <c r="C58" s="25" t="s">
@@ -2023,27 +2038,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A59" s="27">
-        <v>36</v>
-      </c>
-      <c r="B59" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="C59" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="D59" s="25"/>
-      <c r="E59" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="F59" s="25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A60" s="22">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" s="22">
         <v>37</v>
+      </c>
+      <c r="B59" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C59" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="D59" s="30"/>
+      <c r="E59" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="F59" s="30">
+        <v>4</v>
+      </c>
+      <c r="K59">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" s="29">
+        <v>38</v>
       </c>
       <c r="B60" s="30" t="s">
         <v>103</v>
@@ -2053,33 +2071,39 @@
       </c>
       <c r="D60" s="30"/>
       <c r="E60" s="30" t="s">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="F60" s="30">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="K60">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="29">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B61" s="30" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C61" s="30" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D61" s="30"/>
       <c r="E61" s="30" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F61" s="30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="K61">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="29">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B62" s="30" t="s">
         <v>108</v>
@@ -2089,27 +2113,28 @@
       </c>
       <c r="D62" s="30"/>
       <c r="E62" s="30" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="F62" s="30">
         <v>4</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A63" s="29">
-        <v>40</v>
-      </c>
-      <c r="B63" s="30" t="s">
-        <v>110</v>
-      </c>
+      <c r="K62">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B63" s="30"/>
       <c r="C63" s="30" t="s">
         <v>111</v>
       </c>
       <c r="D63" s="30"/>
       <c r="E63" s="30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F63" s="30">
+        <v>4</v>
+      </c>
+      <c r="K63">
         <v>4</v>
       </c>
     </row>

</xml_diff>